<commit_message>
[Pipette] Transformer PL 정리
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/1_Schematic/Plasma_Gen_Transformer_Part List_V1.0.xlsx
+++ b/1_Plasma_Pipette/1_Schematic/Plasma_Gen_Transformer_Part List_V1.0.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171116_Plasma_Generator\1_Plasma_Pipette\1_Schematic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="28035" windowHeight="12780"/>
   </bookViews>
@@ -15,14 +10,14 @@
     <sheet name="Plasma_Gen_Transformer_SCH_V1.0" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Plasma_Gen_Transformer_SCH_V1.0!$B$5:$R$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Plasma_Gen_Transformer_SCH_V1.0!$B$6:$R$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="97">
   <si>
     <t>No</t>
   </si>
@@ -66,9 +61,6 @@
     <t>220uF 16V ALUMINUM CAPACITORS 6.3pi</t>
   </si>
   <si>
-    <t>C16</t>
-  </si>
-  <si>
     <t>7.7mm</t>
   </si>
   <si>
@@ -90,9 +82,6 @@
     <t>CAP CER 0.1uF 16V 10% X7R 0402</t>
   </si>
   <si>
-    <t>C21</t>
-  </si>
-  <si>
     <t>0.55mm</t>
   </si>
   <si>
@@ -114,9 +103,6 @@
     <t>RES SMD 100K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t>R2,R3</t>
-  </si>
-  <si>
     <t>0.40mm</t>
   </si>
   <si>
@@ -129,9 +115,6 @@
     <t>Power MOSFET 40V, Single N-Channel, 101A DPAK</t>
   </si>
   <si>
-    <t>Q1,Q5</t>
-  </si>
-  <si>
     <t>2.38mm</t>
   </si>
   <si>
@@ -168,16 +151,10 @@
     <t>CTX2106XX-R</t>
   </si>
   <si>
-    <t>CTX210605-R</t>
-  </si>
-  <si>
     <t>COOPER Bussmann</t>
   </si>
   <si>
     <t>TRANSFORMER CCFL 6W</t>
-  </si>
-  <si>
-    <t>TX3</t>
   </si>
   <si>
     <t>7.1mm</t>
@@ -246,6 +223,120 @@
   </si>
   <si>
     <t>2,2,2</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVMFS5C450NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semiconductor </t>
+  </si>
+  <si>
+    <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
+  </si>
+  <si>
+    <t>Q1,Q2</t>
+  </si>
+  <si>
+    <t>T491D227K016AT</t>
+  </si>
+  <si>
+    <t>220uF/16V</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>Tantal Capacitor 220uF/16V Case-D 7343 size</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C1</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>C3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>C6</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>C4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1,R2</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3,R4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>R5,R6</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q3,Q4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q5,Q6</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>J3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>J1</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX1</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX2</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB Solder PAD 3x3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTX210609-R</t>
+  </si>
+  <si>
+    <t>Type A</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type B</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type C</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -647,7 +738,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -942,6 +1033,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1103,7 +1233,7 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1298,6 +1428,91 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="48" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="33" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="48" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="19" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="23" xfId="46" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="21" fillId="33" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="14" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="14" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="14" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - 강조색1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1361,9 +1576,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1411,7 +1623,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1446,7 +1658,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1655,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R21"/>
+  <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23:K24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1671,7 +1883,8 @@
     <col min="6" max="6" width="49.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9" style="19"/>
+    <col min="10" max="10" width="9.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="19"/>
     <col min="12" max="12" width="9" style="27"/>
     <col min="13" max="13" width="14.75" style="46" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.75" style="46" customWidth="1"/>
@@ -1682,7 +1895,7 @@
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H1" s="45"/>
       <c r="J1" s="20"/>
@@ -1691,194 +1904,152 @@
       <c r="M1" s="45"/>
       <c r="N1" s="45"/>
     </row>
-    <row r="4" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:18" s="85" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+    </row>
     <row r="5" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="86" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H6" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="23" t="s">
+      <c r="I6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="N6" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="31">
+        <v>1</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="39">
+        <v>1</v>
+      </c>
+      <c r="I7" s="41">
+        <v>90</v>
+      </c>
+      <c r="J7" s="41">
+        <f>H7*I7</f>
+        <v>90</v>
+      </c>
+      <c r="K7" s="30">
+        <v>10</v>
+      </c>
+      <c r="L7" s="41">
+        <f t="shared" ref="L7:L12" si="0">IF(H7&gt;K7,H7*I7,K7*I7)</f>
+        <v>900</v>
+      </c>
+      <c r="M7" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q5" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="31">
-        <v>1</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="N7" s="57">
+        <v>50</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="30" t="s">
+      <c r="R7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="39">
-        <v>1</v>
-      </c>
-      <c r="I6" s="41">
-        <v>90</v>
-      </c>
-      <c r="J6" s="41">
-        <f>H6*I6</f>
-        <v>90</v>
-      </c>
-      <c r="K6" s="30">
-        <v>10</v>
-      </c>
-      <c r="L6" s="41">
-        <f t="shared" ref="L6:L11" si="0">IF(H6&gt;K6,H6*I6,K6*I6)</f>
-        <v>900</v>
-      </c>
-      <c r="M6" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="57">
-        <v>50</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="29">
-        <v>2</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="47">
-        <v>1</v>
-      </c>
-      <c r="I7" s="38">
-        <v>10</v>
-      </c>
-      <c r="J7" s="38">
-        <f>H7*I7</f>
-        <v>10</v>
-      </c>
-      <c r="K7" s="33">
-        <v>100</v>
-      </c>
-      <c r="L7" s="38">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R7" s="34" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="91" t="s">
+        <v>20</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="H8" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="38">
         <v>10</v>
       </c>
       <c r="J8" s="38">
-        <f t="shared" ref="J8:J11" si="1">H8*I8</f>
-        <v>20</v>
+        <f>H8*I8</f>
+        <v>10</v>
       </c>
       <c r="K8" s="33">
         <v>100</v>
@@ -1890,379 +2061,1276 @@
       <c r="M8" s="8"/>
       <c r="N8" s="58"/>
       <c r="O8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="R8" s="34" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="F9" s="91" t="s">
+        <v>27</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="H9" s="47">
         <v>2</v>
       </c>
       <c r="I9" s="38">
+        <v>10</v>
+      </c>
+      <c r="J9" s="38">
+        <f t="shared" ref="J9:J12" si="1">H9*I9</f>
+        <v>20</v>
+      </c>
+      <c r="K9" s="33">
+        <v>100</v>
+      </c>
+      <c r="L9" s="38">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="29">
+        <v>4</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="47">
+        <v>2</v>
+      </c>
+      <c r="I10" s="38">
         <v>1260</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J10" s="38">
         <f t="shared" si="1"/>
         <v>2520</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K10" s="33">
         <v>1</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L10" s="38">
         <f t="shared" si="0"/>
         <v>2520</v>
       </c>
-      <c r="M9" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="N9" s="9">
+      <c r="M10" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="9">
         <v>10</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="33" t="s">
+      <c r="O10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="R9" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="29">
+      <c r="Q10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="29">
         <v>5</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="47">
+      <c r="C11" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="47">
         <v>1</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I11" s="38">
         <v>130</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J11" s="38">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K11" s="33">
         <v>100</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L11" s="38">
         <f t="shared" si="0"/>
         <v>13000</v>
       </c>
-      <c r="M10" s="61" t="s">
+      <c r="M11" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" s="56">
+        <v>100</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="29">
+        <v>6</v>
+      </c>
+      <c r="C12" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="95" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="47">
+        <v>1</v>
+      </c>
+      <c r="I12" s="92">
+        <v>11090</v>
+      </c>
+      <c r="J12" s="38">
+        <f t="shared" si="1"/>
+        <v>11090</v>
+      </c>
+      <c r="K12" s="33">
+        <v>1</v>
+      </c>
+      <c r="L12" s="38">
+        <f t="shared" si="0"/>
+        <v>11090</v>
+      </c>
+      <c r="M12" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="R12" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="26">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="80" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="25">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="35">
+        <f>SUM(J7:J13)</f>
+        <v>13860</v>
+      </c>
+      <c r="L14" s="35">
+        <f>SUM(L7:L13)</f>
+        <v>29510</v>
+      </c>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+    </row>
+    <row r="15" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="45"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+    </row>
+    <row r="16" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" s="37" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="M17" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="O17" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="42">
+        <v>1</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="39">
+        <v>1</v>
+      </c>
+      <c r="I18" s="41">
+        <v>90</v>
+      </c>
+      <c r="J18" s="41">
+        <f>H18*I18</f>
+        <v>90</v>
+      </c>
+      <c r="K18" s="40">
+        <v>10</v>
+      </c>
+      <c r="L18" s="41">
+        <f t="shared" ref="L18:L23" si="2">IF(H18&gt;K18,H18*I18,K18*I18)</f>
+        <v>900</v>
+      </c>
+      <c r="M18" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="57">
+        <v>50</v>
+      </c>
+      <c r="O18" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="29">
+        <v>2</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="47">
+        <v>1</v>
+      </c>
+      <c r="I19" s="38">
+        <v>10</v>
+      </c>
+      <c r="J19" s="38">
+        <f>H19*I19</f>
+        <v>10</v>
+      </c>
+      <c r="K19" s="33">
+        <v>100</v>
+      </c>
+      <c r="L19" s="38">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29">
+        <v>3</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="47">
+        <v>2</v>
+      </c>
+      <c r="I20" s="38">
+        <v>10</v>
+      </c>
+      <c r="J20" s="38">
+        <f t="shared" ref="J20:J23" si="3">H20*I20</f>
+        <v>20</v>
+      </c>
+      <c r="K20" s="33">
+        <v>100</v>
+      </c>
+      <c r="L20" s="38">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q20" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="R20" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" s="87" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="81">
+        <v>4</v>
+      </c>
+      <c r="C21" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="N10" s="56">
+      <c r="E21" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="66">
+        <v>2</v>
+      </c>
+      <c r="I21" s="89">
+        <v>960</v>
+      </c>
+      <c r="J21" s="68">
+        <f t="shared" si="3"/>
+        <v>1920</v>
+      </c>
+      <c r="K21" s="51">
+        <v>1</v>
+      </c>
+      <c r="L21" s="68">
+        <f t="shared" si="2"/>
+        <v>1920</v>
+      </c>
+      <c r="M21" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" s="78">
+        <v>10</v>
+      </c>
+      <c r="O21" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="P21" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q21" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="29">
+        <v>5</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="47">
+        <v>1</v>
+      </c>
+      <c r="I22" s="38">
+        <v>130</v>
+      </c>
+      <c r="J22" s="38">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="K22" s="33">
         <v>100</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="L22" s="38">
+        <f t="shared" si="2"/>
+        <v>13000</v>
+      </c>
+      <c r="M22" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" s="56">
+        <v>100</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q22" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="29">
+        <v>6</v>
+      </c>
+      <c r="C23" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="95" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="47">
+        <v>1</v>
+      </c>
+      <c r="I23" s="93">
+        <v>11090</v>
+      </c>
+      <c r="J23" s="38">
+        <f t="shared" si="3"/>
+        <v>11090</v>
+      </c>
+      <c r="K23" s="33">
+        <v>1</v>
+      </c>
+      <c r="L23" s="38">
+        <f t="shared" si="2"/>
+        <v>11090</v>
+      </c>
+      <c r="M23" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q23" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q10" s="33" t="s">
+      <c r="R23" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" s="37" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="26">
+        <v>7</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="25">
+        <v>1</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J25" s="35">
+        <f>SUM(J18:J24)</f>
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" s="85" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+    </row>
+    <row r="27" spans="2:18" s="85" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+    </row>
+    <row r="28" spans="2:18" s="84" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J28" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="L28" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="M28" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="O28" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="P28" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q28" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" s="87" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="69">
+        <v>1</v>
+      </c>
+      <c r="C29" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="70">
+        <v>1</v>
+      </c>
+      <c r="I29" s="71">
+        <v>2280</v>
+      </c>
+      <c r="J29" s="71">
+        <f>H29*I29</f>
+        <v>2280</v>
+      </c>
+      <c r="K29" s="72">
+        <v>5</v>
+      </c>
+      <c r="L29" s="71">
+        <f t="shared" ref="L29:L34" si="4">IF(H29&gt;K29,H29*I29,K29*I29)</f>
+        <v>11400</v>
+      </c>
+      <c r="M29" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="N29" s="75">
+        <v>50</v>
+      </c>
+      <c r="O29" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="P29" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="29">
+        <v>2</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="47">
+        <v>1</v>
+      </c>
+      <c r="I30" s="38">
+        <v>10</v>
+      </c>
+      <c r="J30" s="38">
+        <f>H30*I30</f>
+        <v>10</v>
+      </c>
+      <c r="K30" s="33">
+        <v>100</v>
+      </c>
+      <c r="L30" s="38">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R30" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="29">
+        <v>3</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" s="47">
+        <v>2</v>
+      </c>
+      <c r="I31" s="38">
+        <v>10</v>
+      </c>
+      <c r="J31" s="38">
+        <f t="shared" ref="J31:J34" si="5">H31*I31</f>
+        <v>20</v>
+      </c>
+      <c r="K31" s="33">
+        <v>100</v>
+      </c>
+      <c r="L31" s="38">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q31" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="R31" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" s="87" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="81">
+        <v>4</v>
+      </c>
+      <c r="C32" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="H32" s="66">
+        <v>2</v>
+      </c>
+      <c r="I32" s="89">
+        <v>960</v>
+      </c>
+      <c r="J32" s="68">
+        <f t="shared" si="5"/>
+        <v>1920</v>
+      </c>
+      <c r="K32" s="51">
+        <v>1</v>
+      </c>
+      <c r="L32" s="68">
+        <f t="shared" si="4"/>
+        <v>1920</v>
+      </c>
+      <c r="M32" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="N32" s="78">
+        <v>10</v>
+      </c>
+      <c r="O32" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="P32" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q32" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="29">
+        <v>5</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="47">
+        <v>1</v>
+      </c>
+      <c r="I33" s="38">
+        <v>130</v>
+      </c>
+      <c r="J33" s="38">
+        <f t="shared" si="5"/>
+        <v>130</v>
+      </c>
+      <c r="K33" s="33">
+        <v>100</v>
+      </c>
+      <c r="L33" s="38">
+        <f t="shared" si="4"/>
+        <v>13000</v>
+      </c>
+      <c r="M33" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="N33" s="56">
+        <v>100</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q33" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="R33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="6" t="s">
+    </row>
+    <row r="34" spans="2:18" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="29">
+        <v>6</v>
+      </c>
+      <c r="C34" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="95" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" s="47">
+        <v>1</v>
+      </c>
+      <c r="I34" s="94">
+        <v>11090</v>
+      </c>
+      <c r="J34" s="38">
+        <f t="shared" si="5"/>
+        <v>11090</v>
+      </c>
+      <c r="K34" s="33">
+        <v>1</v>
+      </c>
+      <c r="L34" s="38">
+        <f t="shared" si="4"/>
+        <v>11090</v>
+      </c>
+      <c r="M34" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q34" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="R34" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" s="84" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="26">
+        <v>7</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="25">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R35" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="29">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J36" s="35">
+        <f>SUM(J29:J35)</f>
+        <v>15450</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="2:18" s="37" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="47">
+      <c r="H38" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="L38" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="N38" s="64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B39" s="42">
         <v>1</v>
       </c>
-      <c r="I11" s="38">
-        <v>13596</v>
-      </c>
-      <c r="J11" s="38">
-        <f t="shared" si="1"/>
-        <v>13596</v>
-      </c>
-      <c r="K11" s="33">
+      <c r="C39" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="39">
         <v>1</v>
       </c>
-      <c r="L11" s="38">
-        <f t="shared" si="0"/>
-        <v>13596</v>
-      </c>
-      <c r="M11" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q11" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="R11" s="51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="26">
-        <v>6</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="25">
-        <v>1</v>
-      </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="3" t="s">
+      <c r="I39" s="40">
+        <v>200</v>
+      </c>
+      <c r="J39" s="41">
+        <f t="shared" ref="J39:J40" si="6">H39*I39</f>
+        <v>200</v>
+      </c>
+      <c r="K39" s="40">
+        <v>10</v>
+      </c>
+      <c r="L39" s="41">
+        <f t="shared" ref="L39:L40" si="7">IF(H39&gt;K39,H39*I39,K39*I39)</f>
+        <v>2000</v>
+      </c>
+      <c r="M39" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="N39" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="52">
+        <v>2</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="R12" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="J13" s="35">
-        <f>SUM(J6:J12)</f>
-        <v>16366</v>
-      </c>
-      <c r="L13" s="35">
-        <f>SUM(L6:L12)</f>
-        <v>32016</v>
-      </c>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-    </row>
-    <row r="14" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="45"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-    </row>
-    <row r="17" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="2:14" s="37" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="50" t="s">
+      <c r="G40" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="49">
         <v>4</v>
       </c>
-      <c r="F18" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="M18" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" s="64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="42">
-        <v>1</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="39">
-        <v>1</v>
-      </c>
-      <c r="I19" s="40">
-        <v>200</v>
-      </c>
-      <c r="J19" s="41">
-        <f t="shared" ref="J19:J20" si="2">H19*I19</f>
-        <v>200</v>
-      </c>
-      <c r="K19" s="40">
-        <v>10</v>
-      </c>
-      <c r="L19" s="41">
-        <f t="shared" ref="L19:L20" si="3">IF(H19&gt;K19,H19*I19,K19*I19)</f>
+      <c r="I40" s="48">
+        <v>20</v>
+      </c>
+      <c r="J40" s="43">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="K40" s="48">
+        <v>100</v>
+      </c>
+      <c r="L40" s="43">
+        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
-      <c r="M19" s="59" t="s">
-        <v>67</v>
-      </c>
-      <c r="N19" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="52">
-        <v>2</v>
-      </c>
-      <c r="C20" s="60" t="s">
+      <c r="M40" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="49">
-        <v>4</v>
-      </c>
-      <c r="I20" s="48">
-        <v>20</v>
-      </c>
-      <c r="J20" s="43">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="K20" s="48">
-        <v>100</v>
-      </c>
-      <c r="L20" s="43">
-        <f t="shared" si="3"/>
-        <v>2000</v>
-      </c>
-      <c r="M20" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="N20" s="7">
+      <c r="N40" s="7">
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J21" s="35">
-        <f>SUM(J19:J20)</f>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J41" s="35">
+        <f>SUM(J39:J40)</f>
         <v>280</v>
       </c>
-      <c r="L21" s="35">
-        <f>SUM(L19:L20)</f>
+      <c r="L41" s="35">
+        <f>SUM(L39:L40)</f>
         <v>4000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B5:R5"/>
+  <autoFilter ref="B6:R6"/>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>